<commit_message>
Code Optimized Biletix Screenshots Enabled
</commit_message>
<xml_diff>
--- a/BiletixDatabase.xlsx
+++ b/BiletixDatabase.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,11 +479,16 @@
           <t>website</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Image_Path</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>16</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -491,30 +496,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Resim - Kumsaldaki Kız</t>
+          <t>Bubble Show</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Şato Yazar Sahne </t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Bubble Show</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF67/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>9c3705a2-dc59-4dd7-963b-88f8fdc1e1dd</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -522,11 +531,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>28</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -534,30 +544,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Heykel - Deniz Kabuğu</t>
+          <t>Bubble Show</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Şato Yazar Sahne </t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Bubble Show</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF67/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>9c3705a2-dc59-4dd7-963b-88f8fdc1e1dd</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -565,11 +579,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>30</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -577,30 +592,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Heykel - Bir Fincan Kedi</t>
+          <t>Bubble Show</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Şato Yazar Sahne </t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Bubble Show</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF67/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>9c3705a2-dc59-4dd7-963b-88f8fdc1e1dd</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -608,11 +627,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -620,30 +640,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Resim - Kübik Vazo</t>
+          <t>Bubble Show</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Şato Yazar Sahne </t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Bubble Show</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF67/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>9c3705a2-dc59-4dd7-963b-88f8fdc1e1dd</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -651,11 +675,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -663,30 +688,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Resim - Caretta Caretta</t>
+          <t>Sorun Bende Değil Sende</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Çukurambar Kültür ve Sanat Merkezi </t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Sorun Bende Değil Sende</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF98/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>7a27a7a4-ab9e-426c-af36-b0ec912d1e59</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -694,11 +723,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -706,30 +736,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Heykel - Deniz Kaplumbağası</t>
+          <t>Sorun Bende Değil Sende</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Çukurambar Kültür ve Sanat Merkezi </t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Sorun Bende Değil Sende</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF98/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>7a27a7a4-ab9e-426c-af36-b0ec912d1e59</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -737,11 +771,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>28</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -749,30 +784,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Heykel - Küçük Prens</t>
+          <t>Sorun Bende Değil Sende</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Çukurambar Kültür ve Sanat Merkezi </t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Sorun Bende Değil Sende</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF98/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>7a27a7a4-ab9e-426c-af36-b0ec912d1e59</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -780,11 +819,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>31</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -792,30 +832,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Resim - Bir Bar Taburesi Üstünde</t>
+          <t>Sorun Bende Değil Sende</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Çukurambar Kültür ve Sanat Merkezi </t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Sorun Bende Değil Sende</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF98/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>7a27a7a4-ab9e-426c-af36-b0ec912d1e59</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -823,11 +867,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -835,30 +880,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Resim - Watermelon Lady</t>
+          <t>Masterpiece Ankara Heykel - Deniz Kabuğu</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Masterpiece Ankara </t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Masterpiece Ankara Heykel - Deniz Kabuğu</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/41513/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>99217d93-999b-4502-be55-cf75dfa2b0ec</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -866,11 +915,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -878,30 +928,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Heykel - Saksı Kafa</t>
+          <t>Masterpiece Ankara Resim - Kumsaldaki Kız</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Masterpiece Ankara </t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Masterpiece Ankara Resim - Kumsaldaki Kız</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/41495/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>a4480749-0568-4e1d-9f1c-f25ff4c79952</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -909,11 +963,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -921,30 +976,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Heykel - Mermaid Heykel</t>
+          <t>Göksu Lezzet Atlası</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Göksu No: 5 Sahne </t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Göksu Lezzet Atlası</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4HCG8/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>e5bcb154-cfcb-4e88-a062-6788b0fbfe69</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -952,11 +1011,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -964,30 +1024,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Resim - Büyülü Ay</t>
+          <t>Bir Delinin Hatıra Defteri</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Çukurambar Kültür ve Sanat Merkezi </t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Bir Delinin Hatıra Defteri</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF92/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>b6c02a1e-e9bd-4d34-8ebd-9b1d7c437c53</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -995,11 +1059,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1007,30 +1072,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Resim - Cats</t>
+          <t>The Departed</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> JW Marriott Hotel Ankara </t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>The Departed</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4HMS4/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>8f232052-4995-4f33-879f-5f23ef83b235</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1038,11 +1107,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1050,30 +1120,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Heykel - Avatar</t>
+          <t>Altı Üstü Stand Up Gecesi</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Altı Üstü Bar </t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Altı Üstü Stand Up Gecesi</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4EFBX/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>b4106117-83eb-4752-88ff-2368d3793549</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1081,11 +1155,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>20</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1093,30 +1168,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Heykel - Groot</t>
+          <t>Altı Üstü Stand Up Gecesi</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Altı Üstü Bar </t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Altı Üstü Stand Up Gecesi</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4EFBX/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>b4106117-83eb-4752-88ff-2368d3793549</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1124,11 +1203,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>27</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1136,30 +1216,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Resim - Kübik Kadeh</t>
+          <t>Altı Üstü Stand Up Gecesi</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Altı Üstü Bar </t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Altı Üstü Stand Up Gecesi</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4EFBX/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>b4106117-83eb-4752-88ff-2368d3793549</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1167,11 +1251,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1179,30 +1264,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Resim - Begonville</t>
+          <t>Muhteşem Yüzyıl Quiz Night</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Quito Coffee </t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Muhteşem Yüzyıl Quiz Night</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4EFD4/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>d097f9d6-5cd5-4aad-ae8e-e17c8369e910</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1210,11 +1299,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1222,30 +1312,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Heykel - Tütsü Fare</t>
+          <t>Belki Biraz</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> IF Performance Hall </t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Belki Biraz</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4K815/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>0bcc74eb-963c-4861-b4c3-1b7295587234</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1253,11 +1347,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1265,31 +1360,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara Heykel - Sid
-</t>
+          <t>An Epic Symphony &amp; Gökhan Türkmen</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Oran Açık Hava Sahnesi </t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>An Epic Symphony &amp; Gökhan Türkmen</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4EA68/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>13cad75d-b614-431a-983c-88a8931ddd46</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1297,11 +1395,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1309,30 +1408,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Resim - Wine and Chill</t>
+          <t>Gece Oyunu</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Şato Yazar Sahne </t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Gece Oyunu</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF81/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>2117d81a-2996-4071-95a2-33f70c49e2a8</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1340,11 +1443,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1352,30 +1456,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Resim - Denize Doğru</t>
+          <t>Gece Oyunu</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Şato Yazar Sahne </t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Gece Oyunu</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF81/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>2117d81a-2996-4071-95a2-33f70c49e2a8</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1383,11 +1491,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>19</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1395,30 +1504,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Heykel - Kedi Yanım</t>
+          <t>Gece Oyunu</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Şato Yazar Sahne </t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Gece Oyunu</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF81/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>2117d81a-2996-4071-95a2-33f70c49e2a8</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1426,6 +1539,7 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1438,30 +1552,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Heykel - Bir Fincan Kedi</t>
+          <t>Gece Oyunu</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Şato Yazar Sahne </t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Gece Oyunu</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF81/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>2117d81a-2996-4071-95a2-33f70c49e2a8</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1469,11 +1587,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1481,30 +1600,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr"/>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Masterpiece Ankara Resim - Hold My Hand</t>
+          <t>Masterpiece Ümitköy Heykel - Bir Fincan Kedi</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Masterpiece Ankara, Ankara </t>
+          <t xml:space="preserve"> Masterpiece Ümitköy </t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Masterpiece Ankara </t>
+          <t>Masterpiece Ümitköy Heykel - Bir Fincan Kedi</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/115442810/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/41333/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>108a0833-e012-48bc-bf12-49c06518aaac</t>
+          <t>d51bdb39-e37d-421d-886c-525240ccc00d</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1512,11 +1635,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1524,30 +1648,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>The Departed</t>
+          <t>Masterpiece Ankara Heykel - Bir Fincan Kedi</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> JW Marriott Hotel Ankara, Ankara </t>
+          <t xml:space="preserve"> Masterpiece Ankara </t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>JW Marriot Açıkhava Sinema Etkinlikleri</t>
+          <t>Masterpiece Ankara Heykel - Bir Fincan Kedi</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/491257056/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/41514/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>3135230a-9f38-4605-9570-2d6616f966e5</t>
+          <t>e8bde17d-5523-4c6e-b195-58068d243d20</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1555,11 +1683,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1567,30 +1696,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Frozen</t>
+          <t>Hipnozcu</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> JW Marriott Hotel Ankara, Ankara </t>
+          <t xml:space="preserve"> Çukurambar Kültür ve Sanat Merkezi </t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>JW Marriot Açıkhava Sinema Etkinlikleri</t>
+          <t>Hipnozcu</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/491257056/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF97/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>3135230a-9f38-4605-9570-2d6616f966e5</t>
+          <t>56ba860b-392e-40bd-8254-57e0e060877f</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1598,11 +1731,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>27</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1610,30 +1744,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr"/>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Ocean's Twelve</t>
+          <t>Hipnozcu</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> JW Marriott Hotel Ankara, Ankara </t>
+          <t xml:space="preserve"> Çukurambar Kültür ve Sanat Merkezi </t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>JW Marriot Açıkhava Sinema Etkinlikleri</t>
+          <t>Hipnozcu</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/491257056/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF97/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>3135230a-9f38-4605-9570-2d6616f966e5</t>
+          <t>56ba860b-392e-40bd-8254-57e0e060877f</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -1641,11 +1779,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1653,30 +1792,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Maleficent</t>
+          <t>Ben Efsaneyim</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> JW Marriott Hotel Ankara, Ankara </t>
+          <t xml:space="preserve"> CSO Ada Ankara Açıkhava </t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>JW Marriot Açıkhava Sinema Etkinlikleri</t>
+          <t>Ben Efsaneyim</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/491257056/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4HM0G/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>3135230a-9f38-4605-9570-2d6616f966e5</t>
+          <t>e88c9b52-4a95-446c-b6f9-f8dfd23d2c34</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -1684,11 +1827,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1696,30 +1840,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr"/>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>The Hangover</t>
+          <t>Hayvan Çiftliği</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> JW Marriott Hotel Ankara, Ankara </t>
+          <t xml:space="preserve"> Şato Yazar Sahne </t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>JW Marriot Açıkhava Sinema Etkinlikleri</t>
+          <t>Hayvan Çiftliği</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/491257056/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF77/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>3135230a-9f38-4605-9570-2d6616f966e5</t>
+          <t>962ba24e-52aa-4068-98e3-93ae3b9d3d3e</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -1727,11 +1875,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>28</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1739,30 +1888,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr"/>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Sherlock Holmes</t>
+          <t>Hayvan Çiftliği</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> JW Marriott Hotel Ankara, Ankara </t>
+          <t xml:space="preserve"> Şato Yazar Sahne </t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>JW Marriot Açıkhava Sinema Etkinlikleri</t>
+          <t>Hayvan Çiftliği</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/491257056/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF77/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>3135230a-9f38-4605-9570-2d6616f966e5</t>
+          <t>962ba24e-52aa-4068-98e3-93ae3b9d3d3e</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -1770,42 +1923,43 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Eylül</t>
+          <t>Ağustos</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
-          <t>The Curious Case Of Benjamin Button</t>
+          <t>Ben Efsaneyim</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> JW Marriott Hotel Ankara, Ankara </t>
+          <t xml:space="preserve"> CSO Ada Ankara Açıkhava, Ankara </t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>JW Marriot Açıkhava Sinema Etkinlikleri</t>
+          <t>CSO Ada Ankara Açıkhava Sinema Etkinlikleri</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/491257056/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik-grup/497608794/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>3135230a-9f38-4605-9570-2d6616f966e5</t>
+          <t>809fc3d0-9ebe-437b-b38c-67b507e66039</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -1813,42 +1967,43 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>17</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Eylül</t>
+          <t>Ağustos</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Örümcek Adam Eve Dönüş Yok (2021)</t>
+          <t>Yukarı Bak</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> JW Marriott Hotel Ankara, Ankara </t>
+          <t xml:space="preserve"> CSO Ada Ankara Açıkhava, Ankara </t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>JW Marriot Açıkhava Sinema Etkinlikleri</t>
+          <t>CSO Ada Ankara Açıkhava Sinema Etkinlikleri</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/491257056/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik-grup/497608794/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>3135230a-9f38-4605-9570-2d6616f966e5</t>
+          <t>809fc3d0-9ebe-437b-b38c-67b507e66039</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -1856,42 +2011,43 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>21</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Eylül</t>
+          <t>Ağustos</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Mad Max: Fury Road</t>
+          <t>Yıldızlararası</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> JW Marriott Hotel Ankara, Ankara </t>
+          <t xml:space="preserve"> CSO Ada Ankara Açıkhava, Ankara </t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>JW Marriot Açıkhava Sinema Etkinlikleri</t>
+          <t>CSO Ada Ankara Açıkhava Sinema Etkinlikleri</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/491257056/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik-grup/497608794/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>3135230a-9f38-4605-9570-2d6616f966e5</t>
+          <t>809fc3d0-9ebe-437b-b38c-67b507e66039</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -1899,11 +2055,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>24</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1914,27 +2071,27 @@
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Belki Biraz</t>
+          <t>Arabalar</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> CSO Ada Ankara Açıkhava, Ankara </t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>CSO Ada Ankara Açıkhava Sinema Etkinlikleri</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik-grup/497608794/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>809fc3d0-9ebe-437b-b38c-67b507e66039</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -1942,11 +2099,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>28</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1957,27 +2115,27 @@
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Bağzıları</t>
+          <t>Kara Şövalye</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> CSO Ada Ankara Açıkhava, Ankara </t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>CSO Ada Ankara Açıkhava Sinema Etkinlikleri</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik-grup/497608794/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>809fc3d0-9ebe-437b-b38c-67b507e66039</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -1985,11 +2143,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1997,30 +2156,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr"/>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Emre Nalbatoğlu</t>
+          <t>Kurtlar Vadisi Quiz Night</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> Coffee Up Bahçelievler </t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>Kurtlar Vadisi Quiz Night</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4EFD2/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>f2440b32-f481-4e11-8bde-c2b541d471d3</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2028,11 +2191,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>29</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2040,30 +2204,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr"/>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Doruk Ören</t>
+          <t>Kurtlar Vadisi Quiz Night</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> Coffee Up Bahçelievler </t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>Kurtlar Vadisi Quiz Night</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4EFD2/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>f2440b32-f481-4e11-8bde-c2b541d471d3</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2071,11 +2239,12 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2083,30 +2252,34 @@
           <t>Ağustos</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr"/>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Adap</t>
+          <t>Mustafa Sağır Stand Up</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> Fade Stage &amp; Coffee </t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>Mustafa Sağır Stand Up</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MAHH/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>307cdb8f-c1f5-49e8-92ba-0d6e3dc49fda</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2114,42 +2287,47 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Eylül</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr"/>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Ayşegül Fırat</t>
+          <t>Aşk Perdesi</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> Çukurambar Kültür ve Sanat Merkezi </t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>Aşk Perdesi</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF99/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>cb1efcb5-d9ad-4c75-afa5-5583cbaf7954</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2157,42 +2335,47 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>18</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Eylül</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr"/>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Batu Akdeniz Akustik</t>
+          <t>Aşk Perdesi</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> Çukurambar Kültür ve Sanat Merkezi </t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>Aşk Perdesi</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF99/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>cb1efcb5-d9ad-4c75-afa5-5583cbaf7954</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2200,42 +2383,47 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>25</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Eylül</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr"/>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Radiohead Unplugged Tribute</t>
+          <t>Aşk Perdesi</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> Çukurambar Kültür ve Sanat Merkezi </t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>Aşk Perdesi</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF99/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>cb1efcb5-d9ad-4c75-afa5-5583cbaf7954</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2243,42 +2431,47 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Eylül</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr"/>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Güncel Gürsel Artıktay</t>
+          <t>Masterpiece Ümitköy Resim - Kübik Vazo</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> Masterpiece Ümitköy </t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>Masterpiece Ümitköy Resim - Kübik Vazo</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/41326/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>8905c3dd-492f-4508-a0e7-6997f3130614</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2286,42 +2479,47 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Eylül</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr"/>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>The Five Horsemen Metallica Tribute</t>
+          <t>Masterpiece Ankara Resim - Kübik Vazo</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> Masterpiece Ankara </t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>Masterpiece Ankara Resim - Kübik Vazo</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/41496/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>5fcb59ed-593d-41ad-abd3-b190d0554c14</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2329,42 +2527,47 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Eylül</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr"/>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Hande Mehan</t>
+          <t>Sorun Bende Değil Sendese</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> Şato Yazar Sahne </t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>Sorun Bende Değil Sendese</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF80/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>dad25ca0-8911-47c7-b371-5d619245b990</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2372,42 +2575,47 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>21</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Eylül</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr"/>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Twin Tribes</t>
+          <t>Sorun Bende Değil Sendese</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> Şato Yazar Sahne </t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>Sorun Bende Değil Sendese</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF80/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>dad25ca0-8911-47c7-b371-5d619245b990</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -2415,42 +2623,47 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>24</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Ekim</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr"/>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>İbrahim Sarıca</t>
+          <t>Sorun Bende Değil Sendese</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> Şato Yazar Sahne </t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>Sorun Bende Değil Sendese</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4MF80/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>dad25ca0-8911-47c7-b371-5d619245b990</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -2458,42 +2671,47 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Ekim</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr"/>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Orkundk</t>
+          <t>Çizmeli Kedi</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> Göksu Parkı Açıkhava Tiyatrosu </t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>Çizmeli Kedi</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4ACBJ/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>2548c167-d62f-45ee-b2cd-505ce326ddef</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -2501,42 +2719,47 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Ekim</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr"/>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Ferman Akgül</t>
+          <t>Prime Time Stan Up</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> Altı Üstü Bar </t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>Prime Time Stan Up</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4EFC8/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>a48a6fd3-5c7d-484b-a114-fada5d0c9905</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -2544,42 +2767,47 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Ekim</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr"/>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Soft Analog</t>
+          <t>Prime Time Stan Up</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> Altı Üstü Bar </t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>Prime Time Stan Up</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4EFC8/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>a48a6fd3-5c7d-484b-a114-fada5d0c9905</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -2587,42 +2815,47 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>29</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Ekim</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr"/>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Sedef Sebuktekin</t>
+          <t>Prime Time Stan Up</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> Altı Üstü Bar </t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>Prime Time Stan Up</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4EFC8/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>a48a6fd3-5c7d-484b-a114-fada5d0c9905</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
@@ -2630,42 +2863,47 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Ekim</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr"/>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Tuana</t>
+          <t>Lafazans Stand Up Gecesi</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> Berlin Cafe Pub </t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>Lafazans Stand Up Gecesi</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4FS27/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>77fd4acb-b851-47b8-b0e9-a96a6fad19ef</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
@@ -2673,42 +2911,47 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Ekim</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr"/>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Rana Türkyılmaz</t>
+          <t>Lafazans Stand Up Gecesi</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
+          <t xml:space="preserve"> Berlin Cafe Pub </t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
+          <t>Lafazans Stand Up Gecesi</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
+          <t>https://www.biletix.com/etkinlik/4FS27/TURKIYE/tr</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
+          <t>77fd4acb-b851-47b8-b0e9-a96a6fad19ef</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -2716,49 +2959,904 @@
           <t>Biletix</t>
         </is>
       </c>
+      <c r="J53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Lafazans Stand Up Gecesi</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Berlin Cafe Pub </t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Lafazans Stand Up Gecesi</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik/4FS27/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>77fd4acb-b851-47b8-b0e9-a96a6fad19ef</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Örümcek Adam</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Göksu Parkı Açıkhava Tiyatrosu </t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Örümcek Adam</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik/4ACBL/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>bf038b7c-3659-45ae-aa43-b3f7857308c4</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Dj Hakan Küfündür İle 90lar &amp; 2000ler Türkçe Pop Parti</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6:45 KK Ankara </t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Dj Hakan Küfündür İle 90lar &amp; 2000ler Türkçe Pop Parti</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik/4HMY8/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>e50c02b9-e59e-4489-8b8a-185d17fcb8d4</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Emir Can İğrek</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> CerModern </t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Emir Can İğrek</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik/4DT76/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>87c360d3-59e4-4d69-bc2f-608960122cdb</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>90lar Türkçe Pop Partisi</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IF Performance Hall Tepe Prime </t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>90lar Türkçe Pop Partisi</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik/4RX72/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>c925a956-7307-4d25-8c11-5c549ccc91cd</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>90lar Türkçe Pop Partisi</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IF Performance Hall Tepe Prime </t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>90lar Türkçe Pop Partisi</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik/4RX72/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>c925a956-7307-4d25-8c11-5c549ccc91cd</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2000'ler Türkçe Pop Partisi  
+</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IF Performance Hall </t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2000'ler Türkçe Pop Partisi  
+</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik/4K813/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>a4be2b08-1f0d-4233-b561-5a6c5adbc27f</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2000'ler Türkçe Pop Partisi  
+</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> IF Performance Hall </t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2000'ler Türkçe Pop Partisi  
+</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik/4K813/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>a4be2b08-1f0d-4233-b561-5a6c5adbc27f</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Dj Hakan Küfündür İle 90lar &amp; 2000ler Türkçe Pop Parti</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6:45 KK Ankara, Ankara </t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>6:45 KK Ankara Etkinlikleri</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik-grup/297836795/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>1bf34caf-dd1a-4dca-8e6b-d42dc8dec85b</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Kafadar</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6:45 KK Ankara, Ankara </t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>6:45 KK Ankara Etkinlikleri</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik-grup/297836795/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>1bf34caf-dd1a-4dca-8e6b-d42dc8dec85b</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">90lar &amp; 2000ler Türkçe Pop Parti - Mansur Ark &amp; Dj Akcan Akdağ
+</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6:45 KK Ankara, Ankara </t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>6:45 KK Ankara Etkinlikleri</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik-grup/297836795/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>1bf34caf-dd1a-4dca-8e6b-d42dc8dec85b</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
           <t>20</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Kasım</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Depeche Mode Party</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> IF Performance Hall, Ankara </t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>IF Performance Hall Tunus Ankara Etkinlikleri</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>https://www.biletix.com/etkinlik-grup/119378171/TURKIYE/tr</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>6d808f28-c2d3-4961-b9ce-3ba803efb6fe</t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>Biletix</t>
-        </is>
-      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Eylül</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Ayçin Asan</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6:45 KK Ankara, Ankara </t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>6:45 KK Ankara Etkinlikleri</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik-grup/297836795/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>1bf34caf-dd1a-4dca-8e6b-d42dc8dec85b</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Eylül</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Kilink</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6:45 KK Ankara, Ankara </t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>6:45 KK Ankara Etkinlikleri</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik-grup/297836795/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>1bf34caf-dd1a-4dca-8e6b-d42dc8dec85b</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Afacanlar Sirki Çocuk Tiyatrosu</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Çukurambar Kültür ve Sanat Merkezi </t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Afacanlar Sirki Çocuk Tiyatrosu</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik/4MF85/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>f191acde-cec7-45d2-ae20-76f2200341bf</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Afacanlar Sirki Çocuk Tiyatrosu</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Çukurambar Kültür ve Sanat Merkezi </t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Afacanlar Sirki Çocuk Tiyatrosu</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik/4MF85/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>f191acde-cec7-45d2-ae20-76f2200341bf</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Bilim Carnavalı AKM</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Çukurambar Kültür ve Sanat Merkezi </t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Bilim Carnavalı AKM</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik/4MFI2/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>0a73af20-0880-4511-ba38-82e076df76bc</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Bilim Carnavalı AKM</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Çukurambar Kültür ve Sanat Merkezi </t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Bilim Carnavalı AKM</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik/4MFI2/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>0a73af20-0880-4511-ba38-82e076df76bc</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Masterpiece Ankara Resim - Caretta Caretta</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Masterpiece Ankara </t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Masterpiece Ankara Resim - Caretta Caretta</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik/41497/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>bf7e8d7f-151c-4ec3-b71e-ab5caffa4763</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Ağustos</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Masterpiece Ankara Resim - Caretta Caretta</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Masterpiece Ankara </t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Masterpiece Ankara Resim - Caretta Caretta</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>https://www.biletix.com/etkinlik/41497/TURKIYE/tr</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>bf7e8d7f-151c-4ec3-b71e-ab5caffa4763</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>Biletix</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>